<commit_message>
made some changes because i was bored - changes to productpage - changes to productdescriptions
</commit_message>
<xml_diff>
--- a/Website/Preseditation-stuff/Website Planung.xlsx
+++ b/Website/Preseditation-stuff/Website Planung.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25809"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://krispel-my.sharepoint.com/personal/patrick_krispel_com/Documents/Dokumente/1_Zli Stuff/Dokumente/alerlei/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ee02a1a8fac5edb5/Desktop/Work/ZLI/JoergoMat/Website/Preseditation-stuff/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="19" documentId="8_{EF5F7CB4-63A3-41A2-8265-B2E29E15982E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CE97B10A-E180-4E0A-8AE1-6AB35033C69B}"/>
   <bookViews>
-    <workbookView xWindow="1584" yWindow="360" windowWidth="20184" windowHeight="11376" xr2:uid="{11A413A0-7277-47A1-8064-1033870BCD5E}"/>
+    <workbookView minimized="1" xWindow="1464" yWindow="1464" windowWidth="17280" windowHeight="8880" xr2:uid="{11A413A0-7277-47A1-8064-1033870BCD5E}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -95,7 +95,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -462,7 +462,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -761,12 +761,12 @@
   <dimension ref="B4:L17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="4" spans="2:12">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
@@ -779,7 +779,7 @@
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
     </row>
-    <row r="5" spans="2:12" ht="15" thickBot="1">
+    <row r="5" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="5" t="s">
         <v>0</v>
       </c>
@@ -798,7 +798,7 @@
       <c r="K5" s="18"/>
       <c r="L5" s="18"/>
     </row>
-    <row r="6" spans="2:12">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B6" s="8" t="s">
         <v>3</v>
       </c>
@@ -817,7 +817,7 @@
       <c r="K6" s="21"/>
       <c r="L6" s="22"/>
     </row>
-    <row r="7" spans="2:12">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B7" s="2"/>
       <c r="C7" s="1"/>
       <c r="D7" s="23"/>
@@ -830,7 +830,7 @@
       <c r="K7" s="24"/>
       <c r="L7" s="25"/>
     </row>
-    <row r="8" spans="2:12">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
         <v>5</v>
       </c>
@@ -849,7 +849,7 @@
       <c r="K8" s="12"/>
       <c r="L8" s="13"/>
     </row>
-    <row r="9" spans="2:12">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B9" s="2"/>
       <c r="C9" s="1"/>
       <c r="D9" s="23"/>
@@ -862,7 +862,7 @@
       <c r="K9" s="24"/>
       <c r="L9" s="25"/>
     </row>
-    <row r="10" spans="2:12">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
         <v>7</v>
       </c>
@@ -881,7 +881,7 @@
       <c r="K10" s="12"/>
       <c r="L10" s="13"/>
     </row>
-    <row r="11" spans="2:12">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B11" s="2"/>
       <c r="C11" s="1"/>
       <c r="D11" s="23"/>
@@ -894,7 +894,7 @@
       <c r="K11" s="24"/>
       <c r="L11" s="25"/>
     </row>
-    <row r="12" spans="2:12">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="s">
         <v>9</v>
       </c>
@@ -913,7 +913,7 @@
       <c r="K12" s="12"/>
       <c r="L12" s="13"/>
     </row>
-    <row r="13" spans="2:12">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B13" s="2"/>
       <c r="C13" s="1"/>
       <c r="D13" s="23"/>
@@ -926,7 +926,7 @@
       <c r="K13" s="24"/>
       <c r="L13" s="25"/>
     </row>
-    <row r="14" spans="2:12">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
         <v>11</v>
       </c>
@@ -945,7 +945,7 @@
       <c r="K14" s="12"/>
       <c r="L14" s="13"/>
     </row>
-    <row r="15" spans="2:12">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B15" s="6"/>
       <c r="C15" s="7"/>
       <c r="D15" s="14"/>
@@ -958,7 +958,7 @@
       <c r="K15" s="15"/>
       <c r="L15" s="16"/>
     </row>
-    <row r="16" spans="2:12">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B16" s="2"/>
       <c r="C16" s="1"/>
       <c r="D16" s="11"/>
@@ -971,7 +971,7 @@
       <c r="K16" s="12"/>
       <c r="L16" s="13"/>
     </row>
-    <row r="17" spans="2:12" ht="15" thickBot="1">
+    <row r="17" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="10"/>
       <c r="C17" s="3"/>
       <c r="D17" s="17"/>

</xml_diff>